<commit_message>
Updated Readme file with test scenarios for execution including subset of Manual and automation. Updated BlazeUIData model to overcome NullPointerException for empty data field values. Updated ChooseFlightPage Class to verify depart and arrives city. Updated ConfirmationPage Class to verify ConfirmationId. Updated FindFlightsPage Class with additonal methods. Updated CreateBooking Test Class with addional tests.
</commit_message>
<xml_diff>
--- a/test_data/BlazeUiData.xlsx
+++ b/test_data/BlazeUiData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\blazedemo-ui-automation\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7577C3D-124C-4C26-B88A-C7B6087C4437}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08521ACF-4CC9-4EF8-8688-6FCE21A20151}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="40">
   <si>
     <t>scenarioName</t>
   </si>
@@ -66,9 +66,6 @@
     <t>rememberMe</t>
   </si>
   <si>
-    <t>Success</t>
-  </si>
-  <si>
     <t>Boston</t>
   </si>
   <si>
@@ -87,16 +84,67 @@
     <t>Karnataka</t>
   </si>
   <si>
+    <t>4356234512344320</t>
+  </si>
+  <si>
+    <t>origin</t>
+  </si>
+  <si>
+    <t>destination</t>
+  </si>
+  <si>
+    <t>BookFlightBostonToRome</t>
+  </si>
+  <si>
+    <t>imageLink</t>
+  </si>
+  <si>
+    <t>ClickImageLink</t>
+  </si>
+  <si>
+    <t>BookFlightSanDiegoToNewYork</t>
+  </si>
+  <si>
+    <t>San Diego</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>Church Street</t>
+  </si>
+  <si>
+    <t>Albany</t>
+  </si>
+  <si>
+    <t>3456087612468760</t>
+  </si>
+  <si>
+    <t>Tom Hanks</t>
+  </si>
+  <si>
+    <t>BookFlightWithMissingDetails</t>
+  </si>
+  <si>
+    <t>Portland</t>
+  </si>
+  <si>
+    <t>Cairo</t>
+  </si>
+  <si>
+    <t>Karlos</t>
+  </si>
+  <si>
+    <t>Brazil</t>
+  </si>
+  <si>
     <t>visa</t>
   </si>
   <si>
-    <t>4356234512344320</t>
-  </si>
-  <si>
-    <t>origin</t>
-  </si>
-  <si>
-    <t>destination</t>
+    <t>dinersclub</t>
+  </si>
+  <si>
+    <t>amex</t>
   </si>
 </sst>
 </file>
@@ -144,7 +192,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -153,6 +201,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -433,21 +482,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="15.21875" customWidth="1"/>
+    <col min="1" max="1" width="20.44140625" customWidth="1"/>
     <col min="2" max="2" width="11.21875" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
     <col min="4" max="4" width="15.44140625" customWidth="1"/>
     <col min="5" max="5" width="11.77734375" customWidth="1"/>
     <col min="6" max="6" width="14.77734375" customWidth="1"/>
-    <col min="10" max="10" width="10.5546875" customWidth="1"/>
+    <col min="10" max="10" width="23.21875" customWidth="1"/>
     <col min="11" max="11" width="18.33203125" customWidth="1"/>
     <col min="12" max="12" width="17.6640625" customWidth="1"/>
     <col min="13" max="13" width="16.33203125" customWidth="1"/>
@@ -455,15 +504,15 @@
     <col min="15" max="15" width="12.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:16">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -501,40 +550,43 @@
       <c r="O1" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="P1" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:16">
       <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>14</v>
-      </c>
-      <c r="C2" t="s">
-        <v>15</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
         <v>16</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>17</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>18</v>
-      </c>
-      <c r="H2" t="s">
-        <v>19</v>
       </c>
       <c r="I2">
         <v>560103</v>
       </c>
       <c r="J2" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L2">
         <v>11</v>
@@ -543,9 +595,102 @@
         <v>2025</v>
       </c>
       <c r="N2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="O2" t="b">
+        <v>1</v>
+      </c>
+      <c r="P2" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I3">
+        <v>10001</v>
+      </c>
+      <c r="J3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="L3">
+        <v>6</v>
+      </c>
+      <c r="M3">
+        <v>2023</v>
+      </c>
+      <c r="N3" t="s">
+        <v>31</v>
+      </c>
+      <c r="O3" t="b">
+        <v>0</v>
+      </c>
+      <c r="P3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4">
+        <v>5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" t="s">
+        <v>36</v>
+      </c>
+      <c r="I4">
+        <v>20502</v>
+      </c>
+      <c r="J4" t="s">
+        <v>39</v>
+      </c>
+      <c r="O4" t="b">
+        <v>0</v>
+      </c>
+      <c r="P4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="P5" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>